<commit_message>
2019-12-18 +Update: Added all .pdfs and changed some docs
</commit_message>
<xml_diff>
--- a/doc/Tracebility_Matrix.xlsx
+++ b/doc/Tracebility_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hagenberg\ESD - FH OOE Hagenberg\1 Semester\ISE1-Uebung\Jukebox-App\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83CA748-04FA-4180-911D-60A5FE1FE74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA903C2E-746D-46F1-857D-A30DA496C9BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>Rahmenbedingungen </t>
   </si>
@@ -45,9 +45,6 @@
     <t>Screenshots der GUI / Konsole </t>
   </si>
   <si>
-    <t xml:space="preserve">Review-Dokumente (Code- und Designreview) </t>
-  </si>
-  <si>
     <t>Teamstruktur / Rollenaufteilung </t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>Tool_Resümee gibt eine Auflistung an den verwendeten Tools an.</t>
   </si>
   <si>
-    <t>Tool_Resümee zieht ein Resümee über die verwendeten Tools.</t>
-  </si>
-  <si>
     <t>Wochenberichte</t>
   </si>
   <si>
@@ -277,6 +271,24 @@
   </si>
   <si>
     <t>Wochenberichte für die einzelnen Wochen.</t>
+  </si>
+  <si>
+    <t>https://github.com/pagdot/Jukebox-App</t>
+  </si>
+  <si>
+    <t>GitHub und GitHub/SourceCode</t>
+  </si>
+  <si>
+    <t>https://github.com/pagdot/Jukebox-App und Junit.html</t>
+  </si>
+  <si>
+    <t>Das Tool_Resümee gibt auskunft darüber welche Entwicklungsumgebung verwendet wurde.</t>
+  </si>
+  <si>
+    <t>Die Unit Tests sind im GitHub Repo hinterlegt.</t>
+  </si>
+  <si>
+    <t>Source Code kann von GitHub geladen werden. (.apk liegt der Abgabe bei.) Jdoc.html gibt eine entsprechende Dokumentation des Sourcecodes an.</t>
   </si>
 </sst>
 </file>
@@ -355,12 +367,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -713,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F34"/>
+  <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,416 +739,449 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="8">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="E17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" t="s">
-        <v>50</v>
-      </c>
       <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F18" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
         <v>73</v>
       </c>
       <c r="F22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="7">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="8">
-        <v>3</v>
-      </c>
-      <c r="F25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s">
-        <v>61</v>
       </c>
       <c r="D27" t="s">
         <v>74</v>
       </c>
+      <c r="F27" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="F29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
         <v>71</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D31" t="s">
         <v>75</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
+      <c r="C33" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="D33" t="s">
         <v>81</v>
       </c>
-      <c r="C34" t="s">
+      <c r="F33" t="s">
         <v>82</v>
-      </c>
-      <c r="D34" t="s">
-        <v>83</v>
-      </c>
-      <c r="F34" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D23" r:id="rId3" xr:uid="{9A7C8F6B-768B-46EB-AD3E-621633F12461}"/>
+    <hyperlink ref="D29" r:id="rId4" xr:uid="{EE171C5A-9191-4528-A85C-F534B664AA91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
2019-12-18 +Update: Reworked documents
</commit_message>
<xml_diff>
--- a/doc/Tracebility_Matrix.xlsx
+++ b/doc/Tracebility_Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hagenberg\ESD - FH OOE Hagenberg\1 Semester\ISE1-Uebung\Jukebox-App\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD43F80-9038-4916-94EA-DCE1BA193F9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DD677F-1459-4634-AD2C-57866ABE1AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
   <si>
     <t>Rahmenbedingungen </t>
   </si>
@@ -102,9 +102,6 @@
     <t>Kapitel</t>
   </si>
   <si>
-    <t>Sämtliche Designentscheidungen </t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>Screenshots bereits in der Bedienungsnaleitung.pdf enthalten und als .png im Image Ordner.</t>
   </si>
   <si>
-    <t>Mobile/SourceCode</t>
-  </si>
-  <si>
     <t>Mobile/Toolchain und Images</t>
   </si>
   <si>
@@ -273,22 +267,31 @@
     <t>https://github.com/pagdot/Jukebox-App</t>
   </si>
   <si>
-    <t>GitHub und GitHub/SourceCode</t>
-  </si>
-  <si>
-    <t>https://github.com/pagdot/Jukebox-App und Junit.html</t>
-  </si>
-  <si>
     <t>Das Tool_Resümee gibt auskunft darüber welche Entwicklungsumgebung verwendet wurde.</t>
   </si>
   <si>
     <t>Die Unit Tests sind im GitHub Repo hinterlegt.</t>
   </si>
   <si>
-    <t>Source Code kann von GitHub geladen werden. (.apk liegt der Abgabe bei.) Jdoc.html gibt eine entsprechende Dokumentation des Sourcecodes an.</t>
-  </si>
-  <si>
     <t>https://trello.com/b/VhfL13As/jukebox-app</t>
+  </si>
+  <si>
+    <t>Mobile/SourceCode/app</t>
+  </si>
+  <si>
+    <t>index.html</t>
+  </si>
+  <si>
+    <t>GitHub und Mobile/SourceCode/app</t>
+  </si>
+  <si>
+    <t>index.html und https://github.com/pagdot/Jukebox-App</t>
+  </si>
+  <si>
+    <t>Source Code kann von GitHub geladen werden. (.apk und index.html liegt der Abgabe bei.)</t>
+  </si>
+  <si>
+    <t>Generierte Code Dokumentation</t>
   </si>
 </sst>
 </file>
@@ -722,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F33"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +752,7 @@
         <v>25</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -763,33 +766,33 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -800,10 +803,10 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -811,16 +814,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -828,16 +831,16 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -845,13 +848,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -859,117 +862,126 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="7">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>50</v>
-      </c>
-      <c r="F11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>53</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>56</v>
+        <v>26</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="F17" t="s">
         <v>57</v>
@@ -977,67 +989,67 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" t="s">
-        <v>72</v>
+        <v>26</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
@@ -1045,145 +1057,139 @@
         <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>82</v>
+        <v>48</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="7">
+        <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="7">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="F30" t="s">
         <v>73</v>
       </c>
-      <c r="F27" t="s">
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D31" t="s">
-        <v>74</v>
-      </c>
-      <c r="F31" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="C32" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="D32" t="s">
         <v>78</v>
       </c>
-      <c r="C33" t="s">
+      <c r="F32" t="s">
         <v>79</v>
-      </c>
-      <c r="D33" t="s">
-        <v>80</v>
-      </c>
-      <c r="F33" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="D8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D23" r:id="rId3" xr:uid="{9A7C8F6B-768B-46EB-AD3E-621633F12461}"/>
-    <hyperlink ref="D29" r:id="rId4" xr:uid="{EE171C5A-9191-4528-A85C-F534B664AA91}"/>
-    <hyperlink ref="D18" r:id="rId5" xr:uid="{ED4052E0-2128-413E-8B2F-3EBFCC0EE919}"/>
-    <hyperlink ref="D19" r:id="rId6" xr:uid="{D2C447E2-987B-4EEF-92D0-086336FD9532}"/>
+    <hyperlink ref="D22" r:id="rId3" xr:uid="{9A7C8F6B-768B-46EB-AD3E-621633F12461}"/>
+    <hyperlink ref="D17" r:id="rId4" xr:uid="{ED4052E0-2128-413E-8B2F-3EBFCC0EE919}"/>
+    <hyperlink ref="D18" r:id="rId5" xr:uid="{D2C447E2-987B-4EEF-92D0-086336FD9532}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added design choices document and updated matrix
</commit_message>
<xml_diff>
--- a/doc/Tracebility_Matrix.xlsx
+++ b/doc/Tracebility_Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hagenberg\ESD - FH OOE Hagenberg\1 Semester\ISE1-Uebung\Jukebox-App\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FH\Jukebox-App\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DD677F-1459-4634-AD2C-57866ABE1AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DDEE9A-3059-4BF8-BDE6-42E76D10CF87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
   <si>
     <t>Rahmenbedingungen </t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>Generierte Code Dokumentation</t>
+  </si>
+  <si>
+    <t>Getroffene Designentscheidungen</t>
+  </si>
+  <si>
+    <t>Mobile/Designentscheidungen</t>
+  </si>
+  <si>
+    <t>Designentscheidungen.pdf</t>
+  </si>
+  <si>
+    <t>Getroffene Designentscheidungen im Projekt</t>
   </si>
 </sst>
 </file>
@@ -388,8 +400,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -405,7 +417,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -725,23 +737,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:F32"/>
+  <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="95.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.1796875" customWidth="1"/>
+    <col min="2" max="2" width="95.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="63.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" customWidth="1"/>
+    <col min="6" max="6" width="57.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="C1" s="5" t="s">
         <v>22</v>
       </c>
@@ -755,7 +767,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
@@ -764,7 +776,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>34</v>
       </c>
@@ -778,7 +790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
@@ -795,7 +807,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
@@ -809,7 +821,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -826,7 +838,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -843,7 +855,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>3</v>
       </c>
@@ -857,7 +869,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
@@ -874,7 +886,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
@@ -891,7 +903,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>47</v>
       </c>
@@ -905,7 +917,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>51</v>
       </c>
@@ -919,7 +931,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
@@ -933,7 +945,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
@@ -947,7 +959,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
@@ -956,7 +968,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
@@ -973,7 +985,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>8</v>
       </c>
@@ -987,7 +999,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1010,7 +1022,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1024,7 +1036,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
@@ -1038,7 +1050,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>60</v>
       </c>
@@ -1052,7 +1064,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1069,7 +1081,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
@@ -1083,7 +1095,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1097,7 +1109,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>10</v>
       </c>
@@ -1111,72 +1123,86 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>86</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>87</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
         <v>16</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>68</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D31" t="s">
         <v>72</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
         <v>76</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>77</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D33" t="s">
         <v>78</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F33" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1199,7 +1225,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1211,7 +1237,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>